<commit_message>
corrigiendo datos de noviembre
</commit_message>
<xml_diff>
--- a/Data/2022/4. Noviembre2022/calculos_finales.xlsx
+++ b/Data/2022/4. Noviembre2022/calculos_finales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\QuantResearch\QuantResearch\Data viz streamlit\Data\2022\4. Noviembre2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\QuantCo_Streamlit\Data\2022\4. Noviembre2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAC04E0-6768-461A-ABA2-FDEAB84976A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A0059A-94E0-4FD1-83D5-34D93B007E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2655" windowWidth="21585" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6765" yWindow="3045" windowWidth="21585" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +596,8 @@
         <v>2.0226407322613271E-2</v>
       </c>
       <c r="H3">
-        <v>8.0905629290453085E-2</v>
+        <f>0.0809056292904531*100</f>
+        <v>8.0905629290453103</v>
       </c>
       <c r="I3" s="8">
         <f>C3+I2</f>
@@ -658,7 +659,8 @@
         <v>2.2323525582606418E-2</v>
       </c>
       <c r="H5">
-        <v>8.9294102330425673E-2</v>
+        <f>0.0892941023304257*100</f>
+        <v>8.9294102330425709</v>
       </c>
       <c r="I5" s="8">
         <f t="shared" si="0"/>
@@ -690,7 +692,8 @@
         <v>-2.9381849041836272E-3</v>
       </c>
       <c r="H6">
-        <v>-1.1752739616734511E-2</v>
+        <f>-0.0117527396167345*100</f>
+        <v>-1.17527396167345</v>
       </c>
       <c r="I6" s="8">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
se corrigen datos de Noviembre en el retorno acumulado
</commit_message>
<xml_diff>
--- a/Data/2022/4. Noviembre2022/calculos_finales.xlsx
+++ b/Data/2022/4. Noviembre2022/calculos_finales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\QuantCo_Streamlit\Data\2022\4. Noviembre2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A0059A-94E0-4FD1-83D5-34D93B007E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F46E1D-0007-401C-8C77-1198DBD3EAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="3045" windowWidth="21585" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="3090" windowWidth="21585" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,10 +627,11 @@
         <v>1.845120911849589</v>
       </c>
       <c r="H4">
-        <v>7.3804836473983553</v>
+        <f t="shared" ref="H4:H6" si="0">0.0809056292904531*100</f>
+        <v>8.0905629290453103</v>
       </c>
       <c r="I4" s="8">
-        <f t="shared" ref="I4:I6" si="0">C4+I3</f>
+        <f t="shared" ref="I4:I6" si="1">C4+I3</f>
         <v>3.8677616441109191</v>
       </c>
     </row>
@@ -659,11 +660,11 @@
         <v>2.2323525582606418E-2</v>
       </c>
       <c r="H5">
-        <f>0.0892941023304257*100</f>
-        <v>8.9294102330425709</v>
+        <f t="shared" si="0"/>
+        <v>8.0905629290453103</v>
       </c>
       <c r="I5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.1001142023715591</v>
       </c>
     </row>
@@ -692,11 +693,11 @@
         <v>-2.9381849041836272E-3</v>
       </c>
       <c r="H6">
-        <f>-0.0117527396167345*100</f>
-        <v>-1.17527396167345</v>
+        <f t="shared" si="0"/>
+        <v>8.0905629290453103</v>
       </c>
       <c r="I6" s="8">
-        <f t="shared" si="0"/>
+        <f>C6+I5</f>
         <v>5.8062957119531964</v>
       </c>
     </row>

</xml_diff>